<commit_message>
Update breakable brick with small mario, fix some logic
</commit_message>
<xml_diff>
--- a/Super_Mario_Bros3/SpacePartioning/Map1-1/ObjectID_Data.xlsx
+++ b/Super_Mario_Bros3/SpacePartioning/Map1-1/ObjectID_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đại học\Năm3\Nhập môn phát triển game\Super_Mario_Bros3\Super_Mario_Bros3\SpacePartioning\Map1-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A881B-ED6B-4B33-A77D-7F0BA854A7A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEF1508-9931-4EEF-B02F-810AE3C3A6B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB204E66-514B-4525-88A2-E8E705752E77}"/>
   </bookViews>
@@ -564,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367FE060-132C-400E-8146-ED86422B7A61}">
   <dimension ref="F1:M1237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="M243" sqref="M243:M1237"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="O202" sqref="O202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -665,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" ref="M8:N71" si="0">L8-2</f>
+        <f t="shared" ref="M8:M71" si="0">L8-2</f>
         <v>2</v>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
         <v>50</v>
       </c>
       <c r="M72" s="1">
-        <f t="shared" ref="M72:N135" si="2">L72-2</f>
+        <f t="shared" ref="M72:M135" si="2">L72-2</f>
         <v>48</v>
       </c>
     </row>
@@ -2912,7 +2912,7 @@
         <v>86</v>
       </c>
       <c r="M136" s="1">
-        <f t="shared" ref="M136:N190" si="4">L136-2</f>
+        <f t="shared" ref="M136:M190" si="4">L136-2</f>
         <v>84</v>
       </c>
     </row>
@@ -3966,22 +3966,23 @@
     </row>
     <row r="201" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F201">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G201">
-        <v>1859</v>
+        <v>1869</v>
       </c>
       <c r="H201">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="I201">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J201">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L201">
-        <v>128</v>
+        <f>L202+1</f>
+        <v>129</v>
       </c>
       <c r="M201" s="1">
         <v>124</v>
@@ -3989,26 +3990,25 @@
     </row>
     <row r="202" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F202">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G202">
-        <v>1869</v>
+        <v>1859</v>
       </c>
       <c r="H202">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I202">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J202">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L202">
-        <f t="shared" ref="L202:L239" si="6">L201+1</f>
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M202" s="1">
-        <f t="shared" ref="M200:N239" si="7">M201+1</f>
+        <f t="shared" ref="M202:M239" si="6">M201+1</f>
         <v>125</v>
       </c>
     </row>
@@ -4115,11 +4115,11 @@
         <v>1</v>
       </c>
       <c r="L214">
+        <f t="shared" ref="L202:L239" si="7">L213+1</f>
+        <v>133</v>
+      </c>
+      <c r="M214" s="1">
         <f t="shared" si="6"/>
-        <v>133</v>
-      </c>
-      <c r="M214" s="1">
-        <f t="shared" si="7"/>
         <v>129</v>
       </c>
     </row>
@@ -4224,11 +4224,11 @@
         <v>2</v>
       </c>
       <c r="L222">
+        <f t="shared" si="7"/>
+        <v>137</v>
+      </c>
+      <c r="M222" s="1">
         <f t="shared" si="6"/>
-        <v>137</v>
-      </c>
-      <c r="M222" s="1">
-        <f t="shared" si="7"/>
         <v>133</v>
       </c>
     </row>
@@ -4249,11 +4249,11 @@
         <v>2</v>
       </c>
       <c r="L223">
+        <f t="shared" si="7"/>
+        <v>138</v>
+      </c>
+      <c r="M223" s="1">
         <f t="shared" si="6"/>
-        <v>138</v>
-      </c>
-      <c r="M223" s="1">
-        <f t="shared" si="7"/>
         <v>134</v>
       </c>
     </row>
@@ -4274,11 +4274,11 @@
         <v>2</v>
       </c>
       <c r="L224">
+        <f t="shared" si="7"/>
+        <v>139</v>
+      </c>
+      <c r="M224" s="1">
         <f t="shared" si="6"/>
-        <v>139</v>
-      </c>
-      <c r="M224" s="1">
-        <f t="shared" si="7"/>
         <v>135</v>
       </c>
     </row>
@@ -4299,11 +4299,11 @@
         <v>2</v>
       </c>
       <c r="L225">
+        <f t="shared" si="7"/>
+        <v>140</v>
+      </c>
+      <c r="M225" s="1">
         <f t="shared" si="6"/>
-        <v>140</v>
-      </c>
-      <c r="M225" s="1">
-        <f t="shared" si="7"/>
         <v>136</v>
       </c>
     </row>
@@ -4324,11 +4324,11 @@
         <v>2</v>
       </c>
       <c r="L226">
+        <f t="shared" si="7"/>
+        <v>141</v>
+      </c>
+      <c r="M226" s="1">
         <f t="shared" si="6"/>
-        <v>141</v>
-      </c>
-      <c r="M226" s="1">
-        <f t="shared" si="7"/>
         <v>137</v>
       </c>
     </row>
@@ -4349,11 +4349,11 @@
         <v>2</v>
       </c>
       <c r="L227">
+        <f t="shared" si="7"/>
+        <v>142</v>
+      </c>
+      <c r="M227" s="1">
         <f t="shared" si="6"/>
-        <v>142</v>
-      </c>
-      <c r="M227" s="1">
-        <f t="shared" si="7"/>
         <v>138</v>
       </c>
     </row>
@@ -4374,11 +4374,11 @@
         <v>2</v>
       </c>
       <c r="L228">
+        <f t="shared" si="7"/>
+        <v>143</v>
+      </c>
+      <c r="M228" s="1">
         <f t="shared" si="6"/>
-        <v>143</v>
-      </c>
-      <c r="M228" s="1">
-        <f t="shared" si="7"/>
         <v>139</v>
       </c>
     </row>
@@ -4399,11 +4399,11 @@
         <v>2</v>
       </c>
       <c r="L229">
+        <f t="shared" si="7"/>
+        <v>144</v>
+      </c>
+      <c r="M229" s="1">
         <f t="shared" si="6"/>
-        <v>144</v>
-      </c>
-      <c r="M229" s="1">
-        <f t="shared" si="7"/>
         <v>140</v>
       </c>
     </row>
@@ -4424,11 +4424,11 @@
         <v>2</v>
       </c>
       <c r="L230">
+        <f t="shared" si="7"/>
+        <v>145</v>
+      </c>
+      <c r="M230" s="1">
         <f t="shared" si="6"/>
-        <v>145</v>
-      </c>
-      <c r="M230" s="1">
-        <f t="shared" si="7"/>
         <v>141</v>
       </c>
     </row>
@@ -4449,11 +4449,11 @@
         <v>2</v>
       </c>
       <c r="L231">
+        <f t="shared" si="7"/>
+        <v>146</v>
+      </c>
+      <c r="M231" s="1">
         <f t="shared" si="6"/>
-        <v>146</v>
-      </c>
-      <c r="M231" s="1">
-        <f t="shared" si="7"/>
         <v>142</v>
       </c>
     </row>
@@ -4474,11 +4474,11 @@
         <v>2</v>
       </c>
       <c r="L232">
+        <f t="shared" si="7"/>
+        <v>147</v>
+      </c>
+      <c r="M232" s="1">
         <f t="shared" si="6"/>
-        <v>147</v>
-      </c>
-      <c r="M232" s="1">
-        <f t="shared" si="7"/>
         <v>143</v>
       </c>
     </row>
@@ -4527,11 +4527,11 @@
         <v>2</v>
       </c>
       <c r="L235">
+        <f t="shared" si="7"/>
+        <v>149</v>
+      </c>
+      <c r="M235" s="1">
         <f t="shared" si="6"/>
-        <v>149</v>
-      </c>
-      <c r="M235" s="1">
-        <f t="shared" si="7"/>
         <v>145</v>
       </c>
     </row>
@@ -4552,11 +4552,11 @@
         <v>2</v>
       </c>
       <c r="L236">
+        <f t="shared" si="7"/>
+        <v>150</v>
+      </c>
+      <c r="M236" s="1">
         <f t="shared" si="6"/>
-        <v>150</v>
-      </c>
-      <c r="M236" s="1">
-        <f t="shared" si="7"/>
         <v>146</v>
       </c>
     </row>
@@ -4600,11 +4600,11 @@
         <v>2</v>
       </c>
       <c r="L239">
+        <f t="shared" si="7"/>
+        <v>152</v>
+      </c>
+      <c r="M239" s="1">
         <f t="shared" si="6"/>
-        <v>152</v>
-      </c>
-      <c r="M239" s="1">
-        <f t="shared" si="7"/>
         <v>148</v>
       </c>
     </row>

</xml_diff>